<commit_message>
Canada Mass Update code changes
</commit_message>
<xml_diff>
--- a/RequestCMR/config/MassCreateTemplateCA.xlsx
+++ b/RequestCMR/config/MassCreateTemplateCA.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JosephRAMOS\Box Sync\Work\05_IBM\Account\IBMA_CMR\Stories\Canada\mass_create\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JosephRAMOS\Box Sync\Work\05_IBM\Account\IBMA_CMR\Stories\Canada\mass_create\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9601AA2F-3A28-46AE-97FC-17CE62234C95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B95E49A-ECF7-4FA7-B39E-7BE15F5C35ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="645" windowWidth="19440" windowHeight="15000" xr2:uid="{5B94F7EE-DC85-4098-8B55-9847CBC9C8DC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5B94F7EE-DC85-4098-8B55-9847CBC9C8DC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Meta" sheetId="2" r:id="rId2"/>
+    <sheet name="Mass Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>CMR No.</t>
   </si>
@@ -129,97 +128,178 @@
     <t>OEM</t>
   </si>
   <si>
-    <t>Install-At
+    <t>Invoice To
 Country (Landed)</t>
   </si>
   <si>
-    <t>Install-At
+    <t>Invoice To
 Number + Street</t>
   </si>
   <si>
-    <t>Install-At
+    <t>Invoice To
 City</t>
   </si>
   <si>
-    <t>Install-At
+    <t>Invoice To
 District</t>
   </si>
   <si>
-    <t>Install-At
+    <t>Invoice To
 State/Province</t>
   </si>
   <si>
-    <t>Install-At
+    <t>Invoice To
 Postal Code</t>
   </si>
   <si>
-    <t>Install-At
+    <t>Invoice To
 Division</t>
   </si>
   <si>
-    <t>Install-At
+    <t>Invoice To
 Department/ Attention</t>
   </si>
   <si>
-    <t>Install-At
+    <t>Invoice To
 Building</t>
   </si>
   <si>
-    <t>Install-At
+    <t>Invoice To
 Floor</t>
   </si>
   <si>
-    <t>Install-At
+    <t>Invoice To
 Office</t>
   </si>
   <si>
-    <t>Install-At
+    <t>Invoice To
 Phone#</t>
   </si>
   <si>
-    <t>Install-At
+    <t>Invoice To
 PostBox</t>
   </si>
   <si>
-    <t>Install-At
+    <t>Invoice To
 PostBox City</t>
   </si>
   <si>
-    <t>Local Customer</t>
-  </si>
-  <si>
-    <t>Commercial Customer</t>
-  </si>
-  <si>
-    <t>lysolie</t>
-  </si>
-  <si>
-    <t>ENG</t>
-  </si>
-  <si>
-    <t>Template Version</t>
-  </si>
-  <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>Validated</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>CMR_NO</t>
-  </si>
-  <si>
-    <t>SCENARIO_TYPE</t>
+    <t>Maintenance Billing
+Country (Landed)</t>
+  </si>
+  <si>
+    <t>Maintenance Billing
+Number + Street</t>
+  </si>
+  <si>
+    <t>Maintenance Billing
+District</t>
+  </si>
+  <si>
+    <t>Maintenance Billing
+State/Province</t>
+  </si>
+  <si>
+    <t>Maintenance Billing
+Postal Code</t>
+  </si>
+  <si>
+    <t>Maintenance Billing
+Division</t>
+  </si>
+  <si>
+    <t>Maintenance Billing
+Department/ Attention</t>
+  </si>
+  <si>
+    <t>Maintenance Billing
+Building</t>
+  </si>
+  <si>
+    <t>Maintenance Billing
+Floor</t>
+  </si>
+  <si>
+    <t>Maintenance Billing
+Office</t>
+  </si>
+  <si>
+    <t>Maintenance Billing
+Phone#</t>
+  </si>
+  <si>
+    <t>Maintenance Billing
+PostBox</t>
+  </si>
+  <si>
+    <t>Maintenance Billing
+PostBox City</t>
+  </si>
+  <si>
+    <t>Install At
+Country (Landed)</t>
+  </si>
+  <si>
+    <t>Install At
+Number + Street</t>
+  </si>
+  <si>
+    <t>Install At
+City</t>
+  </si>
+  <si>
+    <t>Install At
+District</t>
+  </si>
+  <si>
+    <t>Install At
+State/Province</t>
+  </si>
+  <si>
+    <t>Install At
+Postal Code</t>
+  </si>
+  <si>
+    <t>Install At
+Division</t>
+  </si>
+  <si>
+    <t>Install At
+Department/ Attention</t>
+  </si>
+  <si>
+    <t>Install At
+Building</t>
+  </si>
+  <si>
+    <t>Install At
+Floor</t>
+  </si>
+  <si>
+    <t>Install At
+Office</t>
+  </si>
+  <si>
+    <t>Install At
+Phone#</t>
+  </si>
+  <si>
+    <t>Install At
+PostBox</t>
+  </si>
+  <si>
+    <t>Install At
+PostBox City</t>
+  </si>
+  <si>
+    <t>Maintenance Billing City</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,22 +309,26 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,13 +337,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,18 +372,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,250 +707,317 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8646055F-BED8-4B6A-85ED-E70AC0F9E28F}">
-  <dimension ref="A2:DI4"/>
+  <dimension ref="A1:DI7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="44" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="113" width="40.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8" style="5" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="5"/>
+    <col min="14" max="14" width="17.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.88671875" style="5"/>
+    <col min="19" max="19" width="18.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="21.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="44" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.44140625" style="4" customWidth="1"/>
+    <col min="47" max="47" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="19.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="54" max="59" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="16.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="16.44140625" style="4" customWidth="1"/>
+    <col min="62" max="66" width="16.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="19.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="68" max="73" width="16.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="74" max="113" width="40.88671875" style="4" customWidth="1"/>
+    <col min="114" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="1" spans="1:73" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="BB1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="BC1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BH1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BI1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="BJ1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="BK1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="BL1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="BM1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
+      <c r="BR1" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="BS1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="BU1" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="3" spans="1:45" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AR3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS3" s="3" t="s">
-        <v>44</v>
-      </c>
+    <row r="5" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="AT5" s="6"/>
+      <c r="AU5" s="6"/>
+      <c r="AV5" s="6"/>
+      <c r="AW5" s="6"/>
+      <c r="AX5" s="6"/>
+      <c r="AY5" s="6"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>118099</v>
-      </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" t="s">
-        <v>48</v>
-      </c>
+    <row r="6" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="AT6" s="6"/>
+      <c r="AU6" s="6"/>
+      <c r="AV6" s="6"/>
+      <c r="AW6" s="6"/>
+      <c r="AX6" s="6"/>
+      <c r="AY6" s="6"/>
+    </row>
+    <row r="7" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="AT7" s="6"/>
+      <c r="AU7" s="6"/>
+      <c r="AV7" s="6"/>
+      <c r="AW7" s="6"/>
+      <c r="AX7" s="6"/>
+      <c r="AY7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3049368-89D8-4648-AFEA-9FBEE60FED92}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>